<commit_message>
Excel sheets of raw and processed data for each figure in the paper
</commit_message>
<xml_diff>
--- a/Paper statistics analysis on distributed tracing -- full version.xlsx
+++ b/Paper statistics analysis on distributed tracing -- full version.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="32200" windowHeight="16160" activeTab="1"/>
+    <workbookView windowWidth="32200" windowHeight="16160"/>
   </bookViews>
   <sheets>
     <sheet name="Raw data source" sheetId="6" r:id="rId1"/>
@@ -59,7 +59,7 @@
     <t>https://link.springer.com/search?new-search=true&amp;advancedSearch=true&amp;sortBy=relevance&amp;query=%22distributed+tracing%22&amp;title=&amp;contributor=&amp;journal=&amp;date=custom&amp;dateFrom=2020&amp;dateTo=2024</t>
   </si>
   <si>
-    <t>Willey</t>
+    <t>Wiley</t>
   </si>
   <si>
     <t>https://onlinelibrary.wiley.com/action/doSearch?AllField=%22distributed%20tracing%22&amp;ConceptID=68&amp;content=articlesChapters&amp;field1=AllField&amp;target=default&amp;text1=%22distributed%20tracing%22&amp;AfterYear=2024&amp;BeforeYear=2024</t>
@@ -5721,7 +5721,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Willey</c:v>
+                  <c:v>Wiley</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6131,7 +6131,7 @@
                   <c:v>Springer</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Willey</c:v>
+                  <c:v>Wiley</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MDPI</c:v>
@@ -6212,7 +6212,7 @@
                   <c:v>Springer</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Willey</c:v>
+                  <c:v>Wiley</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MDPI</c:v>
@@ -6293,7 +6293,7 @@
                   <c:v>Springer</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Willey</c:v>
+                  <c:v>Wiley</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MDPI</c:v>
@@ -6374,7 +6374,7 @@
                   <c:v>Springer</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Willey</c:v>
+                  <c:v>Wiley</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MDPI</c:v>
@@ -6455,7 +6455,7 @@
                   <c:v>Springer</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Willey</c:v>
+                  <c:v>Wiley</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MDPI</c:v>
@@ -6749,7 +6749,7 @@
                   <c:v>Springer</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Willey</c:v>
+                  <c:v>Wiley</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MDPI</c:v>
@@ -6833,7 +6833,7 @@
                   <c:v>Springer</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Willey</c:v>
+                  <c:v>Wiley</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MDPI</c:v>
@@ -6917,7 +6917,7 @@
                   <c:v>Springer</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Willey</c:v>
+                  <c:v>Wiley</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MDPI</c:v>
@@ -7001,7 +7001,7 @@
                   <c:v>Springer</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Willey</c:v>
+                  <c:v>Wiley</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MDPI</c:v>
@@ -7295,7 +7295,7 @@
                   <c:v>Springer</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Willey</c:v>
+                  <c:v>Wiley</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MDPI</c:v>
@@ -7378,7 +7378,7 @@
                   <c:v>Springer</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Willey</c:v>
+                  <c:v>Wiley</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MDPI</c:v>
@@ -7461,7 +7461,7 @@
                   <c:v>Springer</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Willey</c:v>
+                  <c:v>Wiley</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MDPI</c:v>
@@ -7754,7 +7754,7 @@
                   <c:v>Springer</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Willey</c:v>
+                  <c:v>Wiley</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MDPI</c:v>
@@ -7837,7 +7837,7 @@
                   <c:v>Springer</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Willey</c:v>
+                  <c:v>Wiley</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MDPI</c:v>
@@ -7920,7 +7920,7 @@
                   <c:v>Springer</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Willey</c:v>
+                  <c:v>Wiley</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MDPI</c:v>
@@ -11615,8 +11615,8 @@
   <sheetPr/>
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -11701,8 +11701,8 @@
   <sheetPr/>
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>

</xml_diff>